<commit_message>
Recalibrated solar radiation and potential ET again after making minor changes to temperature-distribution zones to fix an error preventing model from running past 9/12/04
</commit_message>
<xml_diff>
--- a/calibration/ETp_calibration Results.xlsx
+++ b/calibration/ETp_calibration Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jaengott\Documents\Projects\Russian_River\RR_GSFLOW\calibration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EA0E303-C532-42AD-BA7C-23AAD299A6A6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F428D19-E8B4-4083-B9E7-E040A4CE2207}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24528" windowHeight="12300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24530" windowHeight="12300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="pot_et" sheetId="1" r:id="rId1"/>
@@ -39,9 +39,6 @@
     <t>Measured</t>
   </si>
   <si>
-    <t>Modelled</t>
-  </si>
-  <si>
     <t>Residual</t>
   </si>
   <si>
@@ -178,6 +175,9 @@
   </si>
   <si>
     <t>Diff %</t>
+  </si>
+  <si>
+    <t>Calculated</t>
   </si>
 </sst>
 </file>
@@ -948,7 +948,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Modelled</c:v>
+                  <c:v>Calculated</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1029,40 +1029,40 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>1.05966</c:v>
+                  <c:v>1.0632699999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.59911</c:v>
+                  <c:v>1.6043700000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.5526300000000002</c:v>
+                  <c:v>2.5549200000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.92536</c:v>
+                  <c:v>3.9320400000000002</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.7134999999999998</c:v>
+                  <c:v>4.7610400000000004</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5.7608699999999997</c:v>
+                  <c:v>5.8380999999999998</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6.5022900000000003</c:v>
+                  <c:v>6.56419</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5.7619999999999996</c:v>
+                  <c:v>5.8052400000000004</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4.58561</c:v>
+                  <c:v>4.59748</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3.0140099999999999</c:v>
+                  <c:v>3.0119400000000001</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.6037699999999999</c:v>
+                  <c:v>1.60216</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.94880799999999998</c:v>
+                  <c:v>0.94841699999999995</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1659,40 +1659,40 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>0.95560400000000001</c:v>
+                  <c:v>0.94959800000000005</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.5184599999999999</c:v>
+                  <c:v>1.51339</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.5018799999999999</c:v>
+                  <c:v>2.4979300000000002</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.0178599999999998</c:v>
+                  <c:v>4.0095499999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.8659299999999996</c:v>
+                  <c:v>4.8249500000000003</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6.0038400000000003</c:v>
+                  <c:v>5.9369800000000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6.2281399999999998</c:v>
+                  <c:v>6.1664099999999999</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5.5374400000000001</c:v>
+                  <c:v>5.4934099999999999</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4.3407600000000004</c:v>
+                  <c:v>4.32585</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.8585400000000001</c:v>
+                  <c:v>2.8588300000000002</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.51891</c:v>
+                  <c:v>1.5223</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.87909400000000004</c:v>
+                  <c:v>0.87506700000000004</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3466,15 +3466,15 @@
   <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3482,24 +3482,24 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
       </c>
       <c r="E1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
         <v>5</v>
-      </c>
-      <c r="B2" t="s">
-        <v>6</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -3508,19 +3508,19 @@
         <v>1</v>
       </c>
       <c r="E2">
-        <v>1.05966</v>
+        <v>1.0632699999999999</v>
       </c>
       <c r="F2" s="1">
         <f>D2-E2</f>
-        <v>-5.9660000000000046E-2</v>
+        <v>-6.3269999999999937E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -3529,19 +3529,19 @@
         <v>1.57</v>
       </c>
       <c r="E3">
-        <v>1.59911</v>
+        <v>1.6043700000000001</v>
       </c>
       <c r="F3" s="1">
         <f t="shared" ref="F3:F25" si="0">D3-E3</f>
-        <v>-2.9109999999999969E-2</v>
+        <v>-3.4370000000000012E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C4">
         <v>3</v>
@@ -3550,19 +3550,19 @@
         <v>2.64</v>
       </c>
       <c r="E4">
-        <v>2.5526300000000002</v>
+        <v>2.5549200000000001</v>
       </c>
       <c r="F4" s="1">
         <f t="shared" si="0"/>
-        <v>8.7369999999999948E-2</v>
+        <v>8.5080000000000044E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C5">
         <v>4</v>
@@ -3571,19 +3571,19 @@
         <v>3.89</v>
       </c>
       <c r="E5">
-        <v>3.92536</v>
+        <v>3.9320400000000002</v>
       </c>
       <c r="F5" s="1">
         <f t="shared" si="0"/>
-        <v>-3.5359999999999836E-2</v>
+        <v>-4.2040000000000077E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C6">
         <v>5</v>
@@ -3592,19 +3592,19 @@
         <v>5.0999999999999996</v>
       </c>
       <c r="E6">
-        <v>4.7134999999999998</v>
+        <v>4.7610400000000004</v>
       </c>
       <c r="F6" s="1">
         <f t="shared" si="0"/>
-        <v>0.38649999999999984</v>
+        <v>0.33895999999999926</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C7">
         <v>6</v>
@@ -3613,19 +3613,19 @@
         <v>6.11</v>
       </c>
       <c r="E7">
-        <v>5.7608699999999997</v>
+        <v>5.8380999999999998</v>
       </c>
       <c r="F7" s="1">
         <f t="shared" si="0"/>
-        <v>0.34913000000000061</v>
+        <v>0.27190000000000047</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C8">
         <v>7</v>
@@ -3634,19 +3634,19 @@
         <v>6.59</v>
       </c>
       <c r="E8">
-        <v>6.5022900000000003</v>
+        <v>6.56419</v>
       </c>
       <c r="F8" s="1">
         <f t="shared" si="0"/>
-        <v>8.7709999999999511E-2</v>
+        <v>2.5809999999999889E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C9">
         <v>8</v>
@@ -3655,19 +3655,19 @@
         <v>5.79</v>
       </c>
       <c r="E9">
-        <v>5.7619999999999996</v>
+        <v>5.8052400000000004</v>
       </c>
       <c r="F9" s="1">
         <f t="shared" si="0"/>
-        <v>2.8000000000000469E-2</v>
+        <v>-1.5240000000000364E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B10" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C10">
         <v>9</v>
@@ -3676,19 +3676,19 @@
         <v>4.4800000000000004</v>
       </c>
       <c r="E10">
-        <v>4.58561</v>
+        <v>4.59748</v>
       </c>
       <c r="F10" s="1">
         <f t="shared" si="0"/>
-        <v>-0.10560999999999954</v>
+        <v>-0.11747999999999958</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B11" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C11">
         <v>10</v>
@@ -3697,19 +3697,19 @@
         <v>2.82</v>
       </c>
       <c r="E11">
-        <v>3.0140099999999999</v>
+        <v>3.0119400000000001</v>
       </c>
       <c r="F11" s="1">
         <f t="shared" si="0"/>
-        <v>-0.19401000000000002</v>
+        <v>-0.19194000000000022</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B12" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C12">
         <v>11</v>
@@ -3718,19 +3718,19 @@
         <v>1.31</v>
       </c>
       <c r="E12">
-        <v>1.6037699999999999</v>
+        <v>1.60216</v>
       </c>
       <c r="F12" s="1">
         <f t="shared" si="0"/>
-        <v>-0.29376999999999986</v>
+        <v>-0.29215999999999998</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B13" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C13">
         <v>12</v>
@@ -3739,19 +3739,19 @@
         <v>0.85</v>
       </c>
       <c r="E13">
-        <v>0.94880799999999998</v>
+        <v>0.94841699999999995</v>
       </c>
       <c r="F13" s="1">
         <f t="shared" si="0"/>
-        <v>-9.8808000000000007E-2</v>
+        <v>-9.8416999999999977E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B14" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C14">
         <v>1</v>
@@ -3760,19 +3760,19 @@
         <v>1.02</v>
       </c>
       <c r="E14">
-        <v>0.95560400000000001</v>
+        <v>0.94959800000000005</v>
       </c>
       <c r="F14" s="1">
         <f t="shared" si="0"/>
-        <v>6.4396000000000009E-2</v>
+        <v>7.0401999999999965E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C15">
         <v>2</v>
@@ -3781,19 +3781,19 @@
         <v>1.55</v>
       </c>
       <c r="E15">
-        <v>1.5184599999999999</v>
+        <v>1.51339</v>
       </c>
       <c r="F15" s="1">
         <f t="shared" si="0"/>
-        <v>3.1540000000000123E-2</v>
+        <v>3.6610000000000031E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B16" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C16">
         <v>3</v>
@@ -3802,19 +3802,19 @@
         <v>2.41</v>
       </c>
       <c r="E16">
-        <v>2.5018799999999999</v>
+        <v>2.4979300000000002</v>
       </c>
       <c r="F16" s="1">
         <f t="shared" si="0"/>
-        <v>-9.187999999999974E-2</v>
+        <v>-8.7930000000000064E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B17" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C17">
         <v>4</v>
@@ -3823,19 +3823,19 @@
         <v>4.05</v>
       </c>
       <c r="E17">
-        <v>4.0178599999999998</v>
+        <v>4.0095499999999999</v>
       </c>
       <c r="F17" s="1">
         <f t="shared" si="0"/>
-        <v>3.2140000000000057E-2</v>
+        <v>4.0449999999999875E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B18" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C18">
         <v>5</v>
@@ -3844,19 +3844,19 @@
         <v>4.49</v>
       </c>
       <c r="E18">
-        <v>4.8659299999999996</v>
+        <v>4.8249500000000003</v>
       </c>
       <c r="F18" s="1">
         <f t="shared" si="0"/>
-        <v>-0.37592999999999943</v>
+        <v>-0.33495000000000008</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B19" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C19">
         <v>6</v>
@@ -3865,19 +3865,19 @@
         <v>5.67</v>
       </c>
       <c r="E19">
-        <v>6.0038400000000003</v>
+        <v>5.9369800000000001</v>
       </c>
       <c r="F19" s="1">
         <f t="shared" si="0"/>
-        <v>-0.33384000000000036</v>
+        <v>-0.26698000000000022</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B20" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C20">
         <v>7</v>
@@ -3886,19 +3886,19 @@
         <v>6.14</v>
       </c>
       <c r="E20">
-        <v>6.2281399999999998</v>
+        <v>6.1664099999999999</v>
       </c>
       <c r="F20" s="1">
         <f t="shared" si="0"/>
-        <v>-8.8140000000000107E-2</v>
+        <v>-2.6410000000000267E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B21" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C21">
         <v>8</v>
@@ -3907,19 +3907,19 @@
         <v>5.51</v>
       </c>
       <c r="E21">
-        <v>5.5374400000000001</v>
+        <v>5.4934099999999999</v>
       </c>
       <c r="F21" s="1">
         <f t="shared" si="0"/>
-        <v>-2.7440000000000353E-2</v>
+        <v>1.6589999999999883E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B22" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C22">
         <v>9</v>
@@ -3928,19 +3928,19 @@
         <v>4.45</v>
       </c>
       <c r="E22">
-        <v>4.3407600000000004</v>
+        <v>4.32585</v>
       </c>
       <c r="F22" s="1">
         <f t="shared" si="0"/>
-        <v>0.10923999999999978</v>
+        <v>0.1241500000000002</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B23" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C23">
         <v>10</v>
@@ -3949,19 +3949,19 @@
         <v>3.06</v>
       </c>
       <c r="E23">
-        <v>2.8585400000000001</v>
+        <v>2.8588300000000002</v>
       </c>
       <c r="F23" s="1">
         <f t="shared" si="0"/>
-        <v>0.20145999999999997</v>
+        <v>0.20116999999999985</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B24" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C24">
         <v>11</v>
@@ -3970,19 +3970,19 @@
         <v>1.83</v>
       </c>
       <c r="E24">
-        <v>1.51891</v>
+        <v>1.5223</v>
       </c>
       <c r="F24" s="1">
         <f t="shared" si="0"/>
-        <v>0.31109000000000009</v>
+        <v>0.30770000000000008</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B25" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C25">
         <v>12</v>
@@ -3991,11 +3991,11 @@
         <v>0.98</v>
       </c>
       <c r="E25">
-        <v>0.87909400000000004</v>
+        <v>0.87506700000000004</v>
       </c>
       <c r="F25" s="1">
         <f t="shared" si="0"/>
-        <v>0.10090599999999994</v>
+        <v>0.10493299999999994</v>
       </c>
     </row>
   </sheetData>
@@ -4009,68 +4009,68 @@
   <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="3" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
       <c r="D1" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E1" s="5"/>
       <c r="F1" s="5"/>
       <c r="G1" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="H1" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="H1" s="5" t="s">
-        <v>49</v>
-      </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" t="s">
         <v>31</v>
-      </c>
-      <c r="B3" t="s">
-        <v>32</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3" t="s">
         <v>31</v>
-      </c>
-      <c r="E3" t="s">
-        <v>32</v>
       </c>
       <c r="F3" s="2"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
         <v>33</v>
       </c>
-      <c r="E4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>34</v>
-      </c>
       <c r="B5" s="4">
-        <v>1.203196E-2</v>
+        <v>1.208357E-2</v>
       </c>
       <c r="C5" s="4"/>
       <c r="D5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E5" s="4">
         <v>1.2218649999999999E-2</v>
@@ -4078,23 +4078,23 @@
       <c r="F5" s="1"/>
       <c r="G5" s="4">
         <f>B5-E5</f>
-        <v>-1.8668999999999977E-4</v>
+        <v>-1.3507999999999923E-4</v>
       </c>
       <c r="H5" s="3">
         <f>(G5/E5)*100</f>
-        <v>-1.5279102028456482</v>
+        <v>-1.1055231142556603</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B6" s="4">
-        <v>1.22063E-2</v>
+        <v>1.2138680000000001E-2</v>
       </c>
       <c r="C6" s="4"/>
       <c r="D6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E6" s="4">
         <v>1.313928E-2</v>
@@ -4102,23 +4102,23 @@
       <c r="F6" s="1"/>
       <c r="G6" s="4">
         <f t="shared" ref="G6:G16" si="0">B6-E6</f>
-        <v>-9.3297999999999992E-4</v>
+        <v>-1.0005999999999991E-3</v>
       </c>
       <c r="H6" s="3">
         <f t="shared" ref="H6:H16" si="1">(G6/E6)*100</f>
-        <v>-7.1006934930985564</v>
+        <v>-7.6153335647006468</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B7" s="4">
-        <v>1.22465E-2</v>
+        <v>1.229123E-2</v>
       </c>
       <c r="C7" s="4"/>
       <c r="D7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E7" s="4">
         <v>1.318925E-2</v>
@@ -4126,23 +4126,23 @@
       <c r="F7" s="1"/>
       <c r="G7" s="4">
         <f t="shared" si="0"/>
-        <v>-9.4274999999999914E-4</v>
+        <v>-8.9801999999999937E-4</v>
       </c>
       <c r="H7" s="3">
         <f t="shared" si="1"/>
-        <v>-7.1478666338116215</v>
+        <v>-6.8087268040260014</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B8" s="4">
-        <v>1.331655E-2</v>
+        <v>1.319057E-2</v>
       </c>
       <c r="C8" s="4"/>
       <c r="D8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E8" s="4">
         <v>1.417011E-2</v>
@@ -4150,23 +4150,23 @@
       <c r="F8" s="1"/>
       <c r="G8" s="4">
         <f t="shared" si="0"/>
-        <v>-8.5355999999999974E-4</v>
+        <v>-9.7953999999999923E-4</v>
       </c>
       <c r="H8" s="3">
         <f t="shared" si="1"/>
-        <v>-6.0236653067619077</v>
+        <v>-6.9127198024574206</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B9" s="4">
-        <v>1.157795E-2</v>
+        <v>1.164974E-2</v>
       </c>
       <c r="C9" s="4"/>
       <c r="D9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E9" s="4">
         <v>1.20838E-2</v>
@@ -4174,23 +4174,23 @@
       <c r="F9" s="1"/>
       <c r="G9" s="4">
         <f t="shared" si="0"/>
-        <v>-5.058500000000004E-4</v>
+        <v>-4.3406E-4</v>
       </c>
       <c r="H9" s="3">
         <f t="shared" si="1"/>
-        <v>-4.1861831543057679</v>
+        <v>-3.5920819609725414</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B10" s="4">
-        <v>1.1607009999999999E-2</v>
+        <v>1.1564359999999999E-2</v>
       </c>
       <c r="C10" s="4"/>
       <c r="D10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E10" s="4">
         <v>1.145463E-2</v>
@@ -4198,23 +4198,23 @@
       <c r="F10" s="1"/>
       <c r="G10" s="4">
         <f t="shared" si="0"/>
-        <v>1.5237999999999884E-4</v>
+        <v>1.0972999999999886E-4</v>
       </c>
       <c r="H10" s="3">
         <f t="shared" si="1"/>
-        <v>1.3302917684813813</v>
+        <v>0.95795324685300931</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B11" s="4">
-        <v>1.1198949999999999E-2</v>
+        <v>1.120386E-2</v>
       </c>
       <c r="C11" s="4"/>
       <c r="D11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E11" s="4">
         <v>1.09818E-2</v>
@@ -4222,23 +4222,23 @@
       <c r="F11" s="1"/>
       <c r="G11" s="4">
         <f t="shared" si="0"/>
-        <v>2.1714999999999929E-4</v>
+        <v>2.2205999999999962E-4</v>
       </c>
       <c r="H11" s="3">
         <f t="shared" si="1"/>
-        <v>1.977362545302221</v>
+        <v>2.0220728842266262</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B12" s="4">
-        <v>1.0963250000000001E-2</v>
+        <v>1.103818E-2</v>
       </c>
       <c r="C12" s="4"/>
       <c r="D12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E12" s="4">
         <v>1.0727520000000001E-2</v>
@@ -4246,23 +4246,23 @@
       <c r="F12" s="1"/>
       <c r="G12" s="4">
         <f t="shared" si="0"/>
-        <v>2.3572999999999997E-4</v>
+        <v>3.1065999999999906E-4</v>
       </c>
       <c r="H12" s="3">
         <f t="shared" si="1"/>
-        <v>2.1974323981684485</v>
+        <v>2.8959162975226245</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B13" s="4">
-        <v>1.141292E-2</v>
+        <v>1.1443470000000001E-2</v>
       </c>
       <c r="C13" s="4"/>
       <c r="D13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E13" s="4">
         <v>1.140591E-2</v>
@@ -4270,23 +4270,23 @@
       <c r="F13" s="1"/>
       <c r="G13" s="4">
         <f t="shared" si="0"/>
-        <v>7.0100000000000023E-6</v>
+        <v>3.7560000000000718E-5</v>
       </c>
       <c r="H13" s="3">
         <f t="shared" si="1"/>
-        <v>6.1459366240834819E-2</v>
+        <v>0.32930296661994279</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B14" s="4">
-        <v>1.256533E-2</v>
+        <v>1.2459609999999999E-2</v>
       </c>
       <c r="C14" s="4"/>
       <c r="D14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E14" s="4">
         <v>1.3155750000000001E-2</v>
@@ -4294,23 +4294,23 @@
       <c r="F14" s="1"/>
       <c r="G14" s="4">
         <f t="shared" si="0"/>
-        <v>-5.9042000000000122E-4</v>
+        <v>-6.9614000000000134E-4</v>
       </c>
       <c r="H14" s="3">
         <f t="shared" si="1"/>
-        <v>-4.4879235315356496</v>
+        <v>-5.291526518822578</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B15" s="4">
-        <v>1.301804E-2</v>
+        <v>1.2828579999999999E-2</v>
       </c>
       <c r="C15" s="4"/>
       <c r="D15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E15" s="4">
         <v>1.359455E-2</v>
@@ -4318,23 +4318,23 @@
       <c r="F15" s="1"/>
       <c r="G15" s="4">
         <f t="shared" si="0"/>
-        <v>-5.7651000000000056E-4</v>
+        <v>-7.6597000000000123E-4</v>
       </c>
       <c r="H15" s="3">
         <f t="shared" si="1"/>
-        <v>-4.2407435332541388</v>
+        <v>-5.6343902519759848</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B16" s="4">
-        <v>1.3152870000000001E-2</v>
+        <v>1.3027209999999999E-2</v>
       </c>
       <c r="C16" s="4"/>
       <c r="D16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E16" s="4">
         <v>1.327688E-2</v>
@@ -4342,11 +4342,11 @@
       <c r="F16" s="1"/>
       <c r="G16" s="4">
         <f t="shared" si="0"/>
-        <v>-1.2400999999999905E-4</v>
+        <v>-2.4967000000000045E-4</v>
       </c>
       <c r="H16" s="3">
         <f t="shared" si="1"/>
-        <v>-0.93402968167219291</v>
+        <v>-1.8804869818812888</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
completed daily SF calibration
</commit_message>
<xml_diff>
--- a/calibration/ETp_calibration Results.xlsx
+++ b/calibration/ETp_calibration Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jaengott\Documents\Projects\Russian_River\RR_GSFLOW\calibration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F428D19-E8B4-4083-B9E7-E040A4CE2207}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55968D34-2014-4B74-8CFE-26CADC6A0EB5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24530" windowHeight="12300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24528" windowHeight="12300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="pot_et" sheetId="1" r:id="rId1"/>
@@ -184,8 +184,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000000000"/>
+    <numFmt numFmtId="173" formatCode="0.00000000"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -664,13 +665,14 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1029,40 +1031,40 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>1.0632699999999999</c:v>
+                  <c:v>1.05627</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.6043700000000001</c:v>
+                  <c:v>1.58876</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.5549200000000001</c:v>
+                  <c:v>2.5140600000000002</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.9320400000000002</c:v>
+                  <c:v>3.8738800000000002</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.7610400000000004</c:v>
+                  <c:v>4.6750400000000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5.8380999999999998</c:v>
+                  <c:v>5.8047399999999998</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6.56419</c:v>
+                  <c:v>6.5459800000000001</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5.8052400000000004</c:v>
+                  <c:v>5.7892299999999999</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4.59748</c:v>
+                  <c:v>4.5906599999999997</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3.0119400000000001</c:v>
+                  <c:v>3.00068</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.60216</c:v>
+                  <c:v>1.5885499999999999</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.94841699999999995</c:v>
+                  <c:v>0.94303899999999996</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1659,40 +1661,40 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>0.94959800000000005</c:v>
+                  <c:v>0.95844300000000004</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.51339</c:v>
+                  <c:v>1.53033</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.4979300000000002</c:v>
+                  <c:v>2.5358000000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.0095499999999999</c:v>
+                  <c:v>4.06616</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.8249500000000003</c:v>
+                  <c:v>4.8962300000000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5.9369800000000001</c:v>
+                  <c:v>5.9665499999999998</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6.1664099999999999</c:v>
+                  <c:v>6.1855099999999998</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5.4934099999999999</c:v>
+                  <c:v>5.5103200000000001</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4.32585</c:v>
+                  <c:v>4.3335100000000004</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.8588300000000002</c:v>
+                  <c:v>2.8722799999999999</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.5223</c:v>
+                  <c:v>1.5430299999999999</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.87506700000000004</c:v>
+                  <c:v>0.88231599999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3469,12 +3471,12 @@
       <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3494,7 +3496,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -3508,14 +3510,14 @@
         <v>1</v>
       </c>
       <c r="E2">
-        <v>1.0632699999999999</v>
+        <v>1.05627</v>
       </c>
       <c r="F2" s="1">
         <f>D2-E2</f>
-        <v>-6.3269999999999937E-2</v>
+        <v>-5.6270000000000042E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -3529,14 +3531,14 @@
         <v>1.57</v>
       </c>
       <c r="E3">
-        <v>1.6043700000000001</v>
+        <v>1.58876</v>
       </c>
       <c r="F3" s="1">
         <f t="shared" ref="F3:F25" si="0">D3-E3</f>
-        <v>-3.4370000000000012E-2</v>
+        <v>-1.8759999999999888E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -3550,14 +3552,14 @@
         <v>2.64</v>
       </c>
       <c r="E4">
-        <v>2.5549200000000001</v>
+        <v>2.5140600000000002</v>
       </c>
       <c r="F4" s="1">
         <f t="shared" si="0"/>
-        <v>8.5080000000000044E-2</v>
+        <v>0.12593999999999994</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -3571,14 +3573,14 @@
         <v>3.89</v>
       </c>
       <c r="E5">
-        <v>3.9320400000000002</v>
+        <v>3.8738800000000002</v>
       </c>
       <c r="F5" s="1">
         <f t="shared" si="0"/>
-        <v>-4.2040000000000077E-2</v>
+        <v>1.6119999999999912E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -3592,14 +3594,14 @@
         <v>5.0999999999999996</v>
       </c>
       <c r="E6">
-        <v>4.7610400000000004</v>
+        <v>4.6750400000000001</v>
       </c>
       <c r="F6" s="1">
         <f t="shared" si="0"/>
-        <v>0.33895999999999926</v>
+        <v>0.42495999999999956</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -3613,14 +3615,14 @@
         <v>6.11</v>
       </c>
       <c r="E7">
-        <v>5.8380999999999998</v>
+        <v>5.8047399999999998</v>
       </c>
       <c r="F7" s="1">
         <f t="shared" si="0"/>
-        <v>0.27190000000000047</v>
+        <v>0.30526000000000053</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -3634,14 +3636,14 @@
         <v>6.59</v>
       </c>
       <c r="E8">
-        <v>6.56419</v>
+        <v>6.5459800000000001</v>
       </c>
       <c r="F8" s="1">
         <f t="shared" si="0"/>
-        <v>2.5809999999999889E-2</v>
+        <v>4.4019999999999726E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -3655,14 +3657,14 @@
         <v>5.79</v>
       </c>
       <c r="E9">
-        <v>5.8052400000000004</v>
+        <v>5.7892299999999999</v>
       </c>
       <c r="F9" s="1">
         <f t="shared" si="0"/>
-        <v>-1.5240000000000364E-2</v>
+        <v>7.7000000000015945E-4</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -3676,14 +3678,14 @@
         <v>4.4800000000000004</v>
       </c>
       <c r="E10">
-        <v>4.59748</v>
+        <v>4.5906599999999997</v>
       </c>
       <c r="F10" s="1">
         <f t="shared" si="0"/>
-        <v>-0.11747999999999958</v>
+        <v>-0.11065999999999931</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -3697,14 +3699,14 @@
         <v>2.82</v>
       </c>
       <c r="E11">
-        <v>3.0119400000000001</v>
+        <v>3.00068</v>
       </c>
       <c r="F11" s="1">
         <f t="shared" si="0"/>
-        <v>-0.19194000000000022</v>
+        <v>-0.18068000000000017</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -3718,14 +3720,14 @@
         <v>1.31</v>
       </c>
       <c r="E12">
-        <v>1.60216</v>
+        <v>1.5885499999999999</v>
       </c>
       <c r="F12" s="1">
         <f t="shared" si="0"/>
-        <v>-0.29215999999999998</v>
+        <v>-0.27854999999999985</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -3739,14 +3741,14 @@
         <v>0.85</v>
       </c>
       <c r="E13">
-        <v>0.94841699999999995</v>
+        <v>0.94303899999999996</v>
       </c>
       <c r="F13" s="1">
         <f t="shared" si="0"/>
-        <v>-9.8416999999999977E-2</v>
+        <v>-9.3038999999999983E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -3760,14 +3762,14 @@
         <v>1.02</v>
       </c>
       <c r="E14">
-        <v>0.94959800000000005</v>
+        <v>0.95844300000000004</v>
       </c>
       <c r="F14" s="1">
         <f t="shared" si="0"/>
-        <v>7.0401999999999965E-2</v>
+        <v>6.1556999999999973E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>18</v>
       </c>
@@ -3781,14 +3783,14 @@
         <v>1.55</v>
       </c>
       <c r="E15">
-        <v>1.51339</v>
+        <v>1.53033</v>
       </c>
       <c r="F15" s="1">
         <f t="shared" si="0"/>
-        <v>3.6610000000000031E-2</v>
+        <v>1.9670000000000076E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>19</v>
       </c>
@@ -3802,14 +3804,14 @@
         <v>2.41</v>
       </c>
       <c r="E16">
-        <v>2.4979300000000002</v>
+        <v>2.5358000000000001</v>
       </c>
       <c r="F16" s="1">
         <f t="shared" si="0"/>
-        <v>-8.7930000000000064E-2</v>
+        <v>-0.12579999999999991</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>20</v>
       </c>
@@ -3823,14 +3825,14 @@
         <v>4.05</v>
       </c>
       <c r="E17">
-        <v>4.0095499999999999</v>
+        <v>4.06616</v>
       </c>
       <c r="F17" s="1">
         <f t="shared" si="0"/>
-        <v>4.0449999999999875E-2</v>
+        <v>-1.6160000000000174E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>21</v>
       </c>
@@ -3844,14 +3846,14 @@
         <v>4.49</v>
       </c>
       <c r="E18">
-        <v>4.8249500000000003</v>
+        <v>4.8962300000000001</v>
       </c>
       <c r="F18" s="1">
         <f t="shared" si="0"/>
-        <v>-0.33495000000000008</v>
+        <v>-0.40622999999999987</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>22</v>
       </c>
@@ -3865,14 +3867,14 @@
         <v>5.67</v>
       </c>
       <c r="E19">
-        <v>5.9369800000000001</v>
+        <v>5.9665499999999998</v>
       </c>
       <c r="F19" s="1">
         <f t="shared" si="0"/>
-        <v>-0.26698000000000022</v>
+        <v>-0.29654999999999987</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>23</v>
       </c>
@@ -3886,14 +3888,14 @@
         <v>6.14</v>
       </c>
       <c r="E20">
-        <v>6.1664099999999999</v>
+        <v>6.1855099999999998</v>
       </c>
       <c r="F20" s="1">
         <f t="shared" si="0"/>
-        <v>-2.6410000000000267E-2</v>
+        <v>-4.5510000000000161E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>24</v>
       </c>
@@ -3907,14 +3909,14 @@
         <v>5.51</v>
       </c>
       <c r="E21">
-        <v>5.4934099999999999</v>
+        <v>5.5103200000000001</v>
       </c>
       <c r="F21" s="1">
         <f t="shared" si="0"/>
-        <v>1.6589999999999883E-2</v>
+        <v>-3.2000000000032003E-4</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>25</v>
       </c>
@@ -3928,14 +3930,14 @@
         <v>4.45</v>
       </c>
       <c r="E22">
-        <v>4.32585</v>
+        <v>4.3335100000000004</v>
       </c>
       <c r="F22" s="1">
         <f t="shared" si="0"/>
-        <v>0.1241500000000002</v>
+        <v>0.11648999999999976</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>26</v>
       </c>
@@ -3949,14 +3951,14 @@
         <v>3.06</v>
       </c>
       <c r="E23">
-        <v>2.8588300000000002</v>
+        <v>2.8722799999999999</v>
       </c>
       <c r="F23" s="1">
         <f t="shared" si="0"/>
-        <v>0.20116999999999985</v>
+        <v>0.18772000000000011</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>27</v>
       </c>
@@ -3970,14 +3972,14 @@
         <v>1.83</v>
       </c>
       <c r="E24">
-        <v>1.5223</v>
+        <v>1.5430299999999999</v>
       </c>
       <c r="F24" s="1">
         <f t="shared" si="0"/>
-        <v>0.30770000000000008</v>
+        <v>0.28697000000000017</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>28</v>
       </c>
@@ -3991,11 +3993,11 @@
         <v>0.98</v>
       </c>
       <c r="E25">
-        <v>0.87506700000000004</v>
+        <v>0.88231599999999999</v>
       </c>
       <c r="F25" s="1">
         <f t="shared" si="0"/>
-        <v>0.10493299999999994</v>
+        <v>9.7683999999999993E-2</v>
       </c>
     </row>
   </sheetData>
@@ -4009,17 +4011,17 @@
   <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="3" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.54296875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>45</v>
       </c>
@@ -4037,7 +4039,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>30</v>
       </c>
@@ -4053,7 +4055,7 @@
       </c>
       <c r="F3" s="2"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>32</v>
       </c>
@@ -4061,292 +4063,292 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>33</v>
       </c>
-      <c r="B5" s="4">
-        <v>1.208357E-2</v>
+      <c r="B5" s="6">
+        <v>1.205229E-2</v>
       </c>
       <c r="C5" s="4"/>
       <c r="D5" t="s">
         <v>33</v>
       </c>
       <c r="E5" s="4">
-        <v>1.2218649999999999E-2</v>
+        <v>1.208357E-2</v>
       </c>
       <c r="F5" s="1"/>
       <c r="G5" s="4">
         <f>B5-E5</f>
-        <v>-1.3507999999999923E-4</v>
+        <v>-3.127999999999985E-5</v>
       </c>
       <c r="H5" s="3">
-        <f>(G5/E5)*100</f>
-        <v>-1.1055231142556603</v>
+        <f>G5/E5</f>
+        <v>-2.5886389535542766E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>34</v>
       </c>
-      <c r="B6" s="4">
-        <v>1.2138680000000001E-2</v>
+      <c r="B6" s="6">
+        <v>1.220924E-2</v>
       </c>
       <c r="C6" s="4"/>
       <c r="D6" t="s">
         <v>34</v>
       </c>
       <c r="E6" s="4">
-        <v>1.313928E-2</v>
+        <v>1.2138680000000001E-2</v>
       </c>
       <c r="F6" s="1"/>
       <c r="G6" s="4">
         <f t="shared" ref="G6:G16" si="0">B6-E6</f>
-        <v>-1.0005999999999991E-3</v>
+        <v>7.0559999999999026E-5</v>
       </c>
       <c r="H6" s="3">
-        <f t="shared" ref="H6:H16" si="1">(G6/E6)*100</f>
-        <v>-7.6153335647006468</v>
+        <f t="shared" ref="H6:H16" si="1">G6/E6</f>
+        <v>5.8128231405720409E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>35</v>
       </c>
-      <c r="B7" s="4">
-        <v>1.229123E-2</v>
+      <c r="B7" s="6">
+        <v>1.22165E-2</v>
       </c>
       <c r="C7" s="4"/>
       <c r="D7" t="s">
         <v>35</v>
       </c>
       <c r="E7" s="4">
-        <v>1.318925E-2</v>
+        <v>1.229123E-2</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="4">
         <f t="shared" si="0"/>
-        <v>-8.9801999999999937E-4</v>
+        <v>-7.4730000000000282E-5</v>
       </c>
       <c r="H7" s="3">
         <f t="shared" si="1"/>
-        <v>-6.8087268040260014</v>
+        <v>-6.0799448061748321E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>36</v>
       </c>
-      <c r="B8" s="4">
-        <v>1.319057E-2</v>
+      <c r="B8" s="6">
+        <v>1.314748E-2</v>
       </c>
       <c r="C8" s="4"/>
       <c r="D8" t="s">
         <v>36</v>
       </c>
       <c r="E8" s="4">
-        <v>1.417011E-2</v>
+        <v>1.319057E-2</v>
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="4">
         <f t="shared" si="0"/>
-        <v>-9.7953999999999923E-4</v>
+        <v>-4.3090000000000836E-5</v>
       </c>
       <c r="H8" s="3">
         <f t="shared" si="1"/>
-        <v>-6.9127198024574206</v>
+        <v>-3.2667276698429889E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>37</v>
       </c>
-      <c r="B9" s="4">
-        <v>1.164974E-2</v>
+      <c r="B9" s="6">
+        <v>1.1468549999999999E-2</v>
       </c>
       <c r="C9" s="4"/>
       <c r="D9" t="s">
         <v>37</v>
       </c>
       <c r="E9" s="4">
-        <v>1.20838E-2</v>
+        <v>1.164974E-2</v>
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="4">
         <f t="shared" si="0"/>
-        <v>-4.3406E-4</v>
+        <v>-1.8119000000000121E-4</v>
       </c>
       <c r="H9" s="3">
         <f t="shared" si="1"/>
-        <v>-3.5920819609725414</v>
+        <v>-1.5553136808203548E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>38</v>
       </c>
-      <c r="B10" s="4">
-        <v>1.1564359999999999E-2</v>
+      <c r="B10" s="6">
+        <v>1.146991E-2</v>
       </c>
       <c r="C10" s="4"/>
       <c r="D10" t="s">
         <v>38</v>
       </c>
       <c r="E10" s="4">
-        <v>1.145463E-2</v>
+        <v>1.1564359999999999E-2</v>
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="4">
         <f t="shared" si="0"/>
-        <v>1.0972999999999886E-4</v>
+        <v>-9.4449999999999396E-5</v>
       </c>
       <c r="H10" s="3">
         <f t="shared" si="1"/>
-        <v>0.95795324685300931</v>
+        <v>-8.1673348114378493E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>39</v>
       </c>
-      <c r="B11" s="4">
-        <v>1.120386E-2</v>
+      <c r="B11" s="6">
+        <v>1.118623E-2</v>
       </c>
       <c r="C11" s="4"/>
       <c r="D11" t="s">
         <v>39</v>
       </c>
       <c r="E11" s="4">
-        <v>1.09818E-2</v>
+        <v>1.120386E-2</v>
       </c>
       <c r="F11" s="1"/>
       <c r="G11" s="4">
         <f t="shared" si="0"/>
-        <v>2.2205999999999962E-4</v>
+        <v>-1.7629999999999382E-5</v>
       </c>
       <c r="H11" s="3">
         <f t="shared" si="1"/>
-        <v>2.0220728842266262</v>
+        <v>-1.5735648249799073E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>40</v>
       </c>
-      <c r="B12" s="4">
-        <v>1.103818E-2</v>
+      <c r="B12" s="6">
+        <v>1.101566E-2</v>
       </c>
       <c r="C12" s="4"/>
       <c r="D12" t="s">
         <v>40</v>
       </c>
       <c r="E12" s="4">
-        <v>1.0727520000000001E-2</v>
+        <v>1.103818E-2</v>
       </c>
       <c r="F12" s="1"/>
       <c r="G12" s="4">
         <f t="shared" si="0"/>
-        <v>3.1065999999999906E-4</v>
+        <v>-2.2519999999999832E-5</v>
       </c>
       <c r="H12" s="3">
         <f t="shared" si="1"/>
-        <v>2.8959162975226245</v>
+        <v>-2.0401914083662191E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>41</v>
       </c>
-      <c r="B13" s="4">
-        <v>1.1443470000000001E-2</v>
+      <c r="B13" s="6">
+        <v>1.1431709999999999E-2</v>
       </c>
       <c r="C13" s="4"/>
       <c r="D13" t="s">
         <v>41</v>
       </c>
       <c r="E13" s="4">
-        <v>1.140591E-2</v>
+        <v>1.1443470000000001E-2</v>
       </c>
       <c r="F13" s="1"/>
       <c r="G13" s="4">
         <f t="shared" si="0"/>
-        <v>3.7560000000000718E-5</v>
+        <v>-1.1760000000001283E-5</v>
       </c>
       <c r="H13" s="3">
         <f t="shared" si="1"/>
-        <v>0.32930296661994279</v>
+        <v>-1.0276603163202492E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>42</v>
       </c>
-      <c r="B14" s="4">
-        <v>1.2459609999999999E-2</v>
+      <c r="B14" s="6">
+        <v>1.2531E-2</v>
       </c>
       <c r="C14" s="4"/>
       <c r="D14" t="s">
         <v>42</v>
       </c>
       <c r="E14" s="4">
-        <v>1.3155750000000001E-2</v>
+        <v>1.2459609999999999E-2</v>
       </c>
       <c r="F14" s="1"/>
       <c r="G14" s="4">
         <f t="shared" si="0"/>
-        <v>-6.9614000000000134E-4</v>
+        <v>7.1390000000001036E-5</v>
       </c>
       <c r="H14" s="3">
         <f t="shared" si="1"/>
-        <v>-5.291526518822578</v>
+        <v>5.7297138513967161E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>43</v>
       </c>
-      <c r="B15" s="4">
-        <v>1.2828579999999999E-2</v>
+      <c r="B15" s="6">
+        <v>1.282899E-2</v>
       </c>
       <c r="C15" s="4"/>
       <c r="D15" t="s">
         <v>43</v>
       </c>
       <c r="E15" s="4">
-        <v>1.359455E-2</v>
+        <v>1.2828579999999999E-2</v>
       </c>
       <c r="F15" s="1"/>
       <c r="G15" s="4">
         <f t="shared" si="0"/>
-        <v>-7.6597000000000123E-4</v>
+        <v>4.1000000000103454E-7</v>
       </c>
       <c r="H15" s="3">
         <f t="shared" si="1"/>
-        <v>-5.6343902519759848</v>
+        <v>3.1959889559174481E-5</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>44</v>
       </c>
-      <c r="B16" s="4">
-        <v>1.3027209999999999E-2</v>
+      <c r="B16" s="6">
+        <v>1.2956809999999999E-2</v>
       </c>
       <c r="C16" s="4"/>
       <c r="D16" t="s">
         <v>44</v>
       </c>
       <c r="E16" s="4">
-        <v>1.327688E-2</v>
+        <v>1.3027209999999999E-2</v>
       </c>
       <c r="F16" s="1"/>
       <c r="G16" s="4">
         <f t="shared" si="0"/>
-        <v>-2.4967000000000045E-4</v>
+        <v>-7.0399999999999976E-5</v>
       </c>
       <c r="H16" s="3">
         <f t="shared" si="1"/>
-        <v>-1.8804869818812888</v>
+        <v>-5.4040734739057694E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>